<commit_message>
Merged all workflows into main branch
</commit_message>
<xml_diff>
--- a/Data/BookingBestChoices.xlsx
+++ b/Data/BookingBestChoices.xlsx
@@ -49,19 +49,19 @@
     <x:t xml:space="preserve">1.311 </x:t>
   </x:si>
   <x:si>
+    <x:t>Vila Sophia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9,8</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">750 </x:t>
+  </x:si>
+  <x:si>
     <x:t>Summer Villa</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">828 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vila Sophia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9,8</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">750 </x:t>
   </x:si>
   <x:si>
     <x:t>PursiSimplu ADULTS ONLY</x:t>
@@ -473,18 +473,18 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>15</x:v>

</xml_diff>